<commit_message>
Testing y arreglos, lista con las cosas que hay que arreglar o faltan.
</commit_message>
<xml_diff>
--- a/Documentacion/Testing y funcionalidades/Testing_Funcionalidades.xlsx
+++ b/Documentacion/Testing y funcionalidades/Testing_Funcionalidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="185">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -495,6 +495,90 @@
   </si>
   <si>
     <t>Datos correctos.</t>
+  </si>
+  <si>
+    <t>dashboard/ver-publicacion-ofrecida/idPublicacion</t>
+  </si>
+  <si>
+    <t>Muestra todos los datos de la publicación.</t>
+  </si>
+  <si>
+    <t>Muestra todos los datos del cliente dueño de la publicación. Muetra puntaje de la publicación y del servicio en general</t>
+  </si>
+  <si>
+    <t>Listado datos de la publicación</t>
+  </si>
+  <si>
+    <t>Listado datos del cliente dueño de la publicación</t>
+  </si>
+  <si>
+    <t>Listado de los comentarios y puntuaciones de la publicación</t>
+  </si>
+  <si>
+    <t>Muestra todos los comentarios y puntajes de la publicación</t>
+  </si>
+  <si>
+    <t>Responder comentario realizado a la publicación</t>
+  </si>
+  <si>
+    <t>Click en link responder. No se ingresa comentario. Solo se responde si es el dueño de la publicación.</t>
+  </si>
+  <si>
+    <t>Click en link responder. Comentario correcto. Solo se responde si es el dueño de la publicación.</t>
+  </si>
+  <si>
+    <t>dashboard/ver-publicacion-solicitada/idPublicacion</t>
+  </si>
+  <si>
+    <t>Listado datos de la solicitud</t>
+  </si>
+  <si>
+    <t>Muestra todos los datos de la solicitud.</t>
+  </si>
+  <si>
+    <t>Muestra imagen y nombre de usuario del cliente dueño de la publicación.</t>
+  </si>
+  <si>
+    <t>FALTA MOSTRAR UBICACIÓN</t>
+  </si>
+  <si>
+    <t>VER LOS PUNTAJES, EL DE LOS SERVICIOS DEBE SER DE SOLICITUDES Y OFERTAS. FALTA MOSTRAR UBICACIÓN</t>
+  </si>
+  <si>
+    <t>Listado de todas las propuestas</t>
+  </si>
+  <si>
+    <t>Muestra todos las propuestas realizadas hasta el momento.</t>
+  </si>
+  <si>
+    <t>Realizar una postulación</t>
+  </si>
+  <si>
+    <t>Click en link postularme. No se ingresa datos.</t>
+  </si>
+  <si>
+    <t>Alert correspondiente indicando que se debe ingresar un texto.</t>
+  </si>
+  <si>
+    <t>Click en link postularme. Datos correctos.</t>
+  </si>
+  <si>
+    <t>Mostrar/Ocultar Propuestas</t>
+  </si>
+  <si>
+    <t>Muestra/Oculta las propuestas realizadas.</t>
+  </si>
+  <si>
+    <t>Aceptar propuesta</t>
+  </si>
+  <si>
+    <t>Click en aceptar propuesta. Unicamente el due;o de la solicitud tiene el link.</t>
+  </si>
+  <si>
+    <t>OK. Se acepta la propuesta, se finaliza la solicitud, se habilita la calificaci'on del usuario contratado.</t>
+  </si>
+  <si>
+    <t>FALTA NOTIFICAR AL CONTRATADO, MOSTRAR DATOS DEL DUE;O DE LA PUBLICACI'ON. MOSTRAR DATOS DEL TRABAJADOR.</t>
   </si>
 </sst>
 </file>
@@ -870,19 +954,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68.5546875" customWidth="1"/>
     <col min="2" max="2" width="50.88671875" customWidth="1"/>
-    <col min="3" max="3" width="99" customWidth="1"/>
+    <col min="3" max="3" width="102.77734375" customWidth="1"/>
     <col min="4" max="4" width="206" customWidth="1"/>
-    <col min="5" max="5" width="76.88671875" customWidth="1"/>
+    <col min="5" max="5" width="108.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2047,7 +2131,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>146</v>
       </c>
@@ -2061,7 +2145,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>146</v>
       </c>
@@ -2075,7 +2159,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>146</v>
       </c>
@@ -2087,6 +2171,197 @@
       </c>
       <c r="D83" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>